<commit_message>
Extra tests and functionality concerning headers
</commit_message>
<xml_diff>
--- a/src/test/resources/test-noproblemsExtraColAndSwitchedCol.xlsx
+++ b/src/test/resources/test-noproblemsExtraColAndSwitchedCol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mephistophilus\MyGitRepositories\ears3\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D1782F-338B-4AA9-9DB9-F4715D75C288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2EBFCF-7509-4112-8C48-BD99FCB8AE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="332" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1493,7 +1493,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1533,11 +1533,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1548,16 +1548,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1597,7 +1587,37 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1608,16 +1628,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1643,31 +1653,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1687,7 +1677,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1697,7 +1687,17 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1773,11 +1773,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1793,11 +1813,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1818,16 +1838,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1858,16 +1868,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1923,6 +1923,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1938,16 +1948,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2073,11 +2073,291 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2143,11 +2423,211 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2188,6 +2668,603 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2317,6 +3394,16 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
@@ -2353,11 +3440,241 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2378,6 +3695,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2443,16 +3780,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2468,6 +3795,46 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2503,21 +3870,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2548,346 +3915,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2943,11 +3970,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2963,11 +3990,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3003,63 +4030,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3075,976 +4045,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10416,11 +10416,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K53">
-    <cfRule type="cellIs" dxfId="254" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="201" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="253" priority="199" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="253" priority="201" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:K31">
@@ -10439,14 +10439,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52">
-    <cfRule type="cellIs" dxfId="249" priority="202" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="249" priority="204" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="248" priority="203" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="204" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="247" priority="202" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K53">
@@ -10473,14 +10473,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K86:K87">
-    <cfRule type="cellIs" dxfId="241" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="75" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="240" priority="73" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="74" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="239" priority="75" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K126:K128">
@@ -10499,22 +10499,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K155:K156 K158:K161">
-    <cfRule type="cellIs" dxfId="235" priority="1189" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="1191" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="234" priority="1189" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="234" priority="1191" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K167:K173">
-    <cfRule type="cellIs" dxfId="233" priority="925" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="233" priority="927" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="232" priority="926" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="231" priority="927" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="231" priority="925" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K174">
@@ -10529,102 +10529,102 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K175:K182">
-    <cfRule type="cellIs" dxfId="227" priority="913" operator="equal">
-      <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="914" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="914" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="915" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="915" operator="equal">
       <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="225" priority="913" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K183">
-    <cfRule type="cellIs" dxfId="224" priority="1138" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="224" priority="1140" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="223" priority="1139" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="1140" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="222" priority="1138" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K184:K193">
-    <cfRule type="cellIs" dxfId="221" priority="895" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="896" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="220" priority="895" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="896" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="219" priority="897" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K194">
-    <cfRule type="cellIs" dxfId="218" priority="1024" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="1025" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="217" priority="1024" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="1025" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="216" priority="1026" operator="equal">
       <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K195:K201">
-    <cfRule type="cellIs" dxfId="215" priority="847" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="848" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="214" priority="847" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="848" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="213" priority="849" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202:K203">
-    <cfRule type="cellIs" dxfId="212" priority="1000" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="1002" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="211" priority="1000" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="1001" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="1001" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="1002" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204:K210">
-    <cfRule type="cellIs" dxfId="209" priority="841" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="209" priority="843" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="208" priority="842" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="843" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="207" priority="841" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="cellIs" dxfId="206" priority="1126" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="1128" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="205" priority="1126" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="1127" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="1127" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="1128" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212:K217 K236:K1048576">
-    <cfRule type="cellIs" dxfId="203" priority="1387" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="1389" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="202" priority="1387" operator="equal">
       <formula>"Interruption"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="1388" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="1388" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="1389" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
@@ -10639,22 +10639,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219:K235">
-    <cfRule type="cellIs" dxfId="197" priority="829" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="830" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="196" priority="829" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="830" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="195" priority="831" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18:L18 K88:L113 K114:K118 L116 L119 K120:K125 L121:L125 K155:K156 K158:L161 L167:L235">
-    <cfRule type="cellIs" dxfId="194" priority="1150" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="1152" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="193" priority="1150" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="1152" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:L48 K133:L154 K127:L127 K18:L18 K88:L113 K114:K118 L116 L119 K120:K125 L121:L125 K155:K156 K158:L161 L167:L235">
@@ -10663,11 +10663,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:L52">
-    <cfRule type="cellIs" dxfId="191" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="210" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="190" priority="208" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="210" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:L36">
@@ -10681,25 +10681,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54:L85">
-    <cfRule type="cellIs" dxfId="187" priority="37" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="187" priority="39" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="186" priority="38" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="39" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="185" priority="37" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K126:L127">
-    <cfRule type="cellIs" dxfId="184" priority="7" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="184" priority="9" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="183" priority="8" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="9" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="182" priority="7" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K129:L134">
@@ -10708,11 +10708,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K129:L154">
-    <cfRule type="cellIs" dxfId="180" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="3" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="179" priority="1" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="3" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K136:L139">
@@ -10721,80 +10721,80 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K166:L166">
-    <cfRule type="cellIs" dxfId="177" priority="262" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="177" priority="264" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="176" priority="263" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="264" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="175" priority="262" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L31">
-    <cfRule type="cellIs" dxfId="174" priority="214" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="174" priority="216" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="173" priority="215" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="216" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="172" priority="214" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52:L53">
-    <cfRule type="cellIs" dxfId="171" priority="196" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="171" priority="198" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="170" priority="197" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="198" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="169" priority="196" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L86:L87">
-    <cfRule type="cellIs" dxfId="168" priority="76" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="168" priority="78" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="167" priority="77" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="78" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="166" priority="76" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L128">
-    <cfRule type="cellIs" dxfId="165" priority="25" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="165" priority="27" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="164" priority="26" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="27" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="163" priority="25" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L138:L139">
     <cfRule type="cellIs" dxfId="162" priority="13" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="15" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="160" priority="14" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="15" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L155:L156">
     <cfRule type="cellIs" dxfId="159" priority="259" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="260" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="261" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="157" priority="260" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="261" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L236:L1048576">
@@ -22366,11 +22366,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA5:AA58">
-    <cfRule type="cellIs" dxfId="151" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="36" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="34" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="36" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27:AA36">
@@ -22389,14 +22389,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA57">
-    <cfRule type="cellIs" dxfId="146" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="39" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="145" priority="37" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="38" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="39" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA58">
@@ -22423,11 +22423,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA91:AA92">
-    <cfRule type="cellIs" dxfId="138" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="25" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="24" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="25" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="136" priority="26" operator="equal">
       <formula>"No impact"</formula>
@@ -22457,69 +22457,69 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA172:AA178">
-    <cfRule type="cellIs" dxfId="130" priority="71" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="130" priority="73" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="129" priority="72" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="73" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="128" priority="71" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA179">
-    <cfRule type="cellIs" dxfId="127" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="90" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="89" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="90" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="125" priority="91" operator="equal">
       <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA180:AA187">
-    <cfRule type="cellIs" dxfId="124" priority="68" operator="equal">
-      <formula>"Interruption"</formula>
+    <cfRule type="cellIs" dxfId="124" priority="70" operator="equal">
+      <formula>"No Impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="123" priority="69" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="70" operator="equal">
-      <formula>"No Impact"</formula>
+    <cfRule type="cellIs" dxfId="122" priority="68" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA188">
-    <cfRule type="cellIs" dxfId="121" priority="86" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="121" priority="88" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="120" priority="87" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="88" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="119" priority="86" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA189:AA198">
-    <cfRule type="cellIs" dxfId="118" priority="65" operator="equal">
-      <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="66" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="67" operator="equal">
       <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="65" operator="equal">
+      <formula>"Interruption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA199">
-    <cfRule type="cellIs" dxfId="115" priority="77" operator="equal">
-      <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="78" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="79" operator="equal">
       <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="77" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA200:AA206">
@@ -22537,11 +22537,11 @@
     <cfRule type="cellIs" dxfId="109" priority="74" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="76" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="75" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="76" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA209:AA215">
@@ -22556,22 +22556,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA216">
-    <cfRule type="cellIs" dxfId="103" priority="83" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="103" priority="85" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="102" priority="84" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="85" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="101" priority="83" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA217:AA222 AA241:AA1048576">
-    <cfRule type="cellIs" dxfId="100" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="102" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="101" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="102" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="98" priority="103" operator="equal">
       <formula>"No Impact"</formula>
@@ -22581,11 +22581,11 @@
     <cfRule type="cellIs" dxfId="97" priority="80" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="82" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="81" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="82" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA224:AA240">
@@ -22600,11 +22600,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA23:AB23 AA93:AB118 AA119:AA123 AB121 AB124 AA125:AA130 AB126:AB130 AA160:AA161 AA163:AB166 AB172:AB240">
-    <cfRule type="cellIs" dxfId="91" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="94" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="92" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="94" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA37:AB53 AA138:AB159 AA132:AB132 AA23:AB23 AA93:AB118 AA119:AA123 AB121 AB124 AA125:AA130 AB126:AB130 AA160:AA161 AA163:AB166 AB172:AB240">
@@ -22613,11 +22613,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA37:AB57">
-    <cfRule type="cellIs" dxfId="88" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="42" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="40" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="42" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA41:AB41">
@@ -22631,25 +22631,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA59:AB90">
-    <cfRule type="cellIs" dxfId="84" priority="20" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="84" priority="22" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="83" priority="21" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="22" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="82" priority="20" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA131:AB132">
-    <cfRule type="cellIs" dxfId="81" priority="8" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="81" priority="10" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="80" priority="9" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="10" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="79" priority="8" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA134:AB139">
@@ -22658,11 +22658,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA134:AB159">
-    <cfRule type="cellIs" dxfId="77" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="4" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="4" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA141:AB144">
@@ -22682,58 +22682,58 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB5:AB36">
-    <cfRule type="cellIs" dxfId="71" priority="44" operator="equal">
-      <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="45" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="46" operator="equal">
       <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="44" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB57:AB58">
-    <cfRule type="cellIs" dxfId="68" priority="31" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="68" priority="33" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="67" priority="32" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="33" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="66" priority="31" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB91:AB92">
-    <cfRule type="cellIs" dxfId="65" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="29" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="27" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="28" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="29" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB133">
-    <cfRule type="cellIs" dxfId="62" priority="17" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="62" priority="19" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="61" priority="18" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="19" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="60" priority="17" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB143:AB144">
-    <cfRule type="cellIs" dxfId="59" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="14" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="12" operator="equal">
       <formula>"Heavy impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="13" operator="equal">
       <formula>"Possible impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="14" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB160:AB161">
@@ -22817,7 +22817,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32260,14 +32260,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB47 AC148:AC1048576">
-    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
-      <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
       <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB48">
@@ -32296,30 +32296,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB141:AB142 AB144:AB147">
-    <cfRule type="cellIs" dxfId="36" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="105" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="103" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="105" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB148:AB1048576">
-    <cfRule type="cellIs" dxfId="34" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="80" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="79" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="80" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="32" priority="81" operator="equal">
       <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB14:AC14 AB82:AC102 AB103:AB107 AC105 AC108 AB109 AB117:AC140 AB141:AB142 AB144:AC147">
-    <cfRule type="cellIs" dxfId="31" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="102" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="100" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="102" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB27:AC43 AB121:AC140 AB115:AC115 AB14:AC14 AB82:AC102 AB103:AB107 AC105 AC108 AB109 AB141:AB142 AB144:AC147">
@@ -32328,11 +32328,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB27:AC47">
-    <cfRule type="cellIs" dxfId="28" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="50" operator="equal">
+      <formula>"No impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="48" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="50" operator="equal">
-      <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB31:AC31">
@@ -32367,66 +32367,66 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:AC26 AB49:AC79 AB80:AB81">
-    <cfRule type="cellIs" dxfId="19" priority="32" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="19" priority="34" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="18" priority="33" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="34" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="17" priority="32" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC47:AC48">
-    <cfRule type="cellIs" dxfId="16" priority="39" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="16" priority="41" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="15" priority="40" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="41" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="14" priority="39" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC80:AC81">
-    <cfRule type="cellIs" dxfId="13" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="36" operator="equal">
+      <formula>"Possible impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="35" operator="equal">
       <formula>"Heavy impact"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="36" operator="equal">
-      <formula>"Possible impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="11" priority="37" operator="equal">
       <formula>"No impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC116">
-    <cfRule type="cellIs" dxfId="10" priority="25" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="10" priority="27" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="9" priority="26" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="8" priority="25" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC125">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
+      <formula>"No Impact"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>"Interruption"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
-      <formula>"No Impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC126:AC127">
-    <cfRule type="cellIs" dxfId="5" priority="20" operator="equal">
-      <formula>"Heavy impact"</formula>
+    <cfRule type="cellIs" dxfId="5" priority="22" operator="equal">
+      <formula>"No impact"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="21" operator="equal">
       <formula>"Possible impact"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="22" operator="equal">
-      <formula>"No impact"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
+      <formula>"Heavy impact"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC141:AC142">

</xml_diff>